<commit_message>
update list MISSING keybinding update
</commit_message>
<xml_diff>
--- a/Visual Studio 2013/Shortcut list.xlsx
+++ b/Visual Studio 2013/Shortcut list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc45be6ccb2f2225/Visual Studio config files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Source\VSConfig\Visual Studio 2013\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Shortcut list</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Alt + Right</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Ctrl + D</t>
   </si>
   <si>
@@ -183,6 +180,39 @@
   </si>
   <si>
     <t>Comment uncomment line</t>
+  </si>
+  <si>
+    <t>Ctrl + Q</t>
+  </si>
+  <si>
+    <t>Quick launch</t>
+  </si>
+  <si>
+    <t>Next highighted</t>
+  </si>
+  <si>
+    <t>Prev highlighted</t>
+  </si>
+  <si>
+    <t>Alt + F12</t>
+  </si>
+  <si>
+    <t>Open code inline editor</t>
+  </si>
+  <si>
+    <t>Ctrl + Space</t>
+  </si>
+  <si>
+    <t>Auto-complete</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + Alt + A</t>
+  </si>
+  <si>
+    <t>Inspect this</t>
+  </si>
+  <si>
+    <t>IMPROVE</t>
   </si>
 </sst>
 </file>
@@ -500,15 +530,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -590,146 +621,184 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>